<commit_message>
New (fixed) excel and tmc for component alarms
</commit_message>
<xml_diff>
--- a/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
+++ b/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markl.BECKHOFF\Source\repos\PML_Base_PLC\PML_Base_PLC_Project\PLC_PML\Base\02_Components\99_EventDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beckhoff_Work\github\PML_Base_PLC\PML_Base_PLC_Project\PLC_PML\Base\02_Components\99_EventDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA135DC-925A-4998-836E-BDCC70B1CD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6F08738D-B868-432B-9E9C-D786710D19A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="2" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Helper" sheetId="4" state="hidden" r:id="rId8"/>
     <sheet name="EventClassHashTable" sheetId="13" state="hidden" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="129">
   <si>
     <t>Key</t>
   </si>
@@ -217,9 +240,6 @@
     <t>{0} - Cylinder command jitter detected - Command cycled between active/inactive within the configured jitter window of {1} ms</t>
   </si>
   <si>
-    <t>InvalidCommand</t>
-  </si>
-  <si>
     <t>{ABE3BB9E-D5A9-46CB-A7C4-C63FD9C74526}</t>
   </si>
   <si>
@@ -334,73 +354,109 @@
     <t>WriteParameterError</t>
   </si>
   <si>
-    <t>MC_Halt Error</t>
-  </si>
-  <si>
-    <t>MC_Power Error</t>
-  </si>
-  <si>
-    <t>MC_Jog Error</t>
-  </si>
-  <si>
-    <t>MC_Reset Error</t>
-  </si>
-  <si>
-    <t>MC_MoveAbsolute Error</t>
-  </si>
-  <si>
-    <t>MC_MoveVelocity Error</t>
-  </si>
-  <si>
-    <t>MC_MoveRelative Error</t>
-  </si>
-  <si>
-    <t>MC_Stop Error</t>
-  </si>
-  <si>
-    <t>MC_Home Error</t>
-  </si>
-  <si>
-    <t>MC_GearIn Error</t>
-  </si>
-  <si>
-    <t>Command Blocked Error</t>
-  </si>
-  <si>
-    <t>Drive Error</t>
-  </si>
-  <si>
-    <t>Write Parameter Error</t>
-  </si>
-  <si>
-    <t>Alpha</t>
-  </si>
-  <si>
-    <t>Timeout While Extending</t>
-  </si>
-  <si>
-    <t>Timeout While Retracting</t>
-  </si>
-  <si>
-    <t>Invalid Command</t>
-  </si>
-  <si>
-    <t>Invalid Position Status / Position Unknown</t>
-  </si>
-  <si>
-    <t>{F8D35679-7848-4050-B739-7C46F9918E40}</t>
-  </si>
-  <si>
-    <t>{B08AAC24-1C6C-457E-A922-E0734E67E0B8}</t>
-  </si>
-  <si>
-    <t>{42F58144-15ED-43AF-B9B8-E08528804F94}</t>
+    <t>{264E72DA-3A30-4083-A2DA-8F96580454DB}</t>
+  </si>
+  <si>
+    <t>AxisError</t>
+  </si>
+  <si>
+    <t>LogicError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_JogError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_PowerError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_ResetError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_MoveAbsoluteError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_MoveVelocityError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_MoveRelativeError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_HaltError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_StopError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_HomeError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_GearInError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_CommandWhileInhibited</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Jog Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis PowerError - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Reset Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Move Position Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Move Velocity Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Move Relative Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Halt Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Stop Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Home Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis Gearing Error - Code: {2}</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis received a motion command while inhibited</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_WriteParameterError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_AxisError</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis failed to write drive parameter</t>
+  </si>
+  <si>
+    <t>{0} - {1} Axis error - Code: {2}</t>
+  </si>
+  <si>
+    <t>DT_ComponentBase_Event_LogicError</t>
+  </si>
+  <si>
+    <t>{0} - Logic error in component - Info: {1}</t>
+  </si>
+  <si>
+    <t>InvalidExtendCommand</t>
+  </si>
+  <si>
+    <t>InvalidRetractCommand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,7 +492,162 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -450,123 +661,123 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Translations" displayName="Translations" ref="A1:K48" totalsRowShown="0">
-  <autoFilter ref="A1:K48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{996F13AF-5004-4345-A522-AEEA959EA73B}" name="Translations" displayName="Translations" ref="A1:K48" totalsRowShown="0">
+  <autoFilter ref="A1:K48" xr:uid="{996F13AF-5004-4345-A522-AEEA959EA73B}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Key"/>
-    <tableColumn id="2" name="German (1031)"/>
-    <tableColumn id="3" name="English (1033)"/>
-    <tableColumn id="4" name="French (1036)"/>
-    <tableColumn id="5" name="Spanish (1034)"/>
-    <tableColumn id="6" name="Dutch (1043)"/>
-    <tableColumn id="7" name="Turkish (1055)"/>
-    <tableColumn id="8" name="Czech (1029)"/>
-    <tableColumn id="9" name="Polish (1045)"/>
-    <tableColumn id="10" name="Russian (1049)"/>
-    <tableColumn id="11" name="Serbian (3098)"/>
+    <tableColumn id="1" xr3:uid="{2837C633-C753-41BA-8BE8-CC58955599E2}" name="Key"/>
+    <tableColumn id="2" xr3:uid="{4F9B8C82-1522-4333-A4E6-0D8108B933FB}" name="German (1031)"/>
+    <tableColumn id="3" xr3:uid="{450EAD45-D88F-49A5-B62E-EF20E47FB18F}" name="English (1033)"/>
+    <tableColumn id="4" xr3:uid="{54AFC46F-5025-4284-820D-DD5890F4BDD2}" name="French (1036)"/>
+    <tableColumn id="5" xr3:uid="{505A646A-D053-4B70-82C9-FFD0B088050F}" name="Spanish (1034)"/>
+    <tableColumn id="6" xr3:uid="{5FDB4755-EAB3-43A6-9AE5-8425F1653EF2}" name="Dutch (1043)"/>
+    <tableColumn id="7" xr3:uid="{B30BBF30-A69C-44DA-9450-145C938200F2}" name="Turkish (1055)"/>
+    <tableColumn id="8" xr3:uid="{98E5DF56-1704-42D1-BDD3-3D9FEFCF1CF9}" name="Czech (1029)"/>
+    <tableColumn id="9" xr3:uid="{D857BD2F-4A55-4E71-9B88-104CC64AD6AF}" name="Polish (1045)"/>
+    <tableColumn id="10" xr3:uid="{C7AF8BC0-5357-4C11-96E0-339648C27463}" name="Russian (1049)"/>
+    <tableColumn id="11" xr3:uid="{95968F16-A063-4007-883C-CEE97FB2E312}" name="Serbian (3098)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="EventClasses" displayName="EventClasses" ref="A1:E41" totalsRowShown="0">
-  <autoFilter ref="A1:E41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70C484A0-1658-4E53-A096-2B7C8DEE4A2F}" name="EventClasses" displayName="EventClasses" ref="A1:E41" totalsRowShown="0">
+  <autoFilter ref="A1:E41" xr:uid="{70C484A0-1658-4E53-A096-2B7C8DEE4A2F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Namespace"/>
-    <tableColumn id="3" name="Guid"/>
-    <tableColumn id="4" name="Display Text"/>
-    <tableColumn id="5" name="Comment"/>
+    <tableColumn id="1" xr3:uid="{5B4ADBFE-41DD-465C-A0D6-AFDB82A42959}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{733EC015-2E60-4093-891A-922F77C94CFF}" name="Namespace"/>
+    <tableColumn id="3" xr3:uid="{61C9FE88-FF30-4CB4-80D2-DA8244B1A88B}" name="Guid"/>
+    <tableColumn id="4" xr3:uid="{66422B65-086C-4014-9848-05A91C98D92D}" name="Display Text"/>
+    <tableColumn id="5" xr3:uid="{A04087B9-3865-4115-A5B0-9AE528C32DE7}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="AxisBase" displayName="AxisBase" ref="A1:E15" totalsRowShown="0">
-  <autoFilter ref="A1:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DDE1A31E-8826-464A-B75B-4BC6DBC7E2E5}" name="AxisBase" displayName="AxisBase" ref="A1:E16" totalsRowShown="0">
+  <autoFilter ref="A1:E16" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Id"/>
-    <tableColumn id="3" name="Severity"/>
-    <tableColumn id="4" name="Display Text"/>
-    <tableColumn id="5" name="Comment"/>
+    <tableColumn id="1" xr3:uid="{D060CB76-1862-4F57-AE75-CC75B3AABFA0}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0AAF161B-4C9C-4C3B-9FA7-271D21F8C2FA}" name="Id"/>
+    <tableColumn id="3" xr3:uid="{64BD8461-609A-4D8A-8BD4-40D60C8D1B50}" name="Severity"/>
+    <tableColumn id="4" xr3:uid="{074786A7-C0BA-4E86-A889-D95D9A369CFC}" name="Display Text"/>
+    <tableColumn id="5" xr3:uid="{E9905B99-60DC-46CB-9F1E-AC0CD2F31517}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="ComponentBase" displayName="ComponentBase" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E270E38A-7D77-4DC9-83C1-9689DC568038}" name="ComponentBase" displayName="ComponentBase" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Id"/>
-    <tableColumn id="3" name="Severity"/>
-    <tableColumn id="4" name="Display Text"/>
-    <tableColumn id="5" name="Comment"/>
+    <tableColumn id="1" xr3:uid="{5ABBF4B5-B987-49AB-9DF1-CD69C5AC9BC6}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{21104FFF-24AC-4D97-8BC1-530416949D8E}" name="Id"/>
+    <tableColumn id="3" xr3:uid="{7F58FFF6-BDED-4D0B-BFD0-140FAD5ABE6F}" name="Severity"/>
+    <tableColumn id="4" xr3:uid="{4B4226C4-FD7A-475F-963A-4B1A519870EF}" name="Display Text"/>
+    <tableColumn id="5" xr3:uid="{37E7FEB1-01D6-4D79-BB16-6946644A1C07}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="CylinderBase" displayName="CylinderBase" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B7344C1E-2E3E-4751-8F12-5B20C8AAD986}" name="CylinderBase" displayName="CylinderBase" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Id"/>
-    <tableColumn id="3" name="Severity"/>
-    <tableColumn id="4" name="Display Text"/>
-    <tableColumn id="5" name="Comment"/>
+    <tableColumn id="1" xr3:uid="{AC4007BC-4546-408A-BBAA-A66332E6BA1B}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{E7144ECE-87CC-48EC-B046-D0ED1A39B0F6}" name="Id"/>
+    <tableColumn id="3" xr3:uid="{8B1C0EF8-E1A4-4819-BC38-7926E617B83D}" name="Severity"/>
+    <tableColumn id="4" xr3:uid="{2D39DC82-11AB-46C9-A9F3-F9F7E4A2A64F}" name="Display Text"/>
+    <tableColumn id="5" xr3:uid="{2634394B-22AB-4F71-9909-7CB09803FD93}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="TemplateEventClass" displayName="TemplateEventClass" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}" name="TemplateEventClass" displayName="TemplateEventClass" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Id"/>
-    <tableColumn id="3" name="Severity"/>
-    <tableColumn id="4" name="Display Text"/>
-    <tableColumn id="5" name="Comment"/>
+    <tableColumn id="1" xr3:uid="{5FE8D805-7213-467A-88B7-2B4A9C2130EA}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{BEB2D209-1204-4B7A-8CE1-B660169C5826}" name="Id"/>
+    <tableColumn id="3" xr3:uid="{A05A5CB2-7071-472D-ADB5-01BED842DA9A}" name="Severity"/>
+    <tableColumn id="4" xr3:uid="{07692664-A866-4D84-B71F-63996025AD45}" name="Display Text"/>
+    <tableColumn id="5" xr3:uid="{EB051D12-2806-4998-8035-7A0316747D05}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B16" totalsRowShown="0">
-  <autoFilter ref="A1:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B14" totalsRowShown="0">
+  <autoFilter ref="A1:B14" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="EventClass"/>
-    <tableColumn id="2" name="Guid"/>
+    <tableColumn id="1" xr3:uid="{04E1E75C-BDF3-4286-A594-63A247B782C9}" name="EventClass"/>
+    <tableColumn id="2" xr3:uid="{49FC7EFD-1932-435E-822B-CCCC5B22F180}" name="Guid"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Helper" displayName="Helper" ref="A1:A6" totalsRowShown="0">
-  <autoFilter ref="A1:A6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{68C70BBF-A60F-459D-BFF4-3BFE573DE5CD}" name="Helper" displayName="Helper" ref="A1:A6" totalsRowShown="0">
+  <autoFilter ref="A1:A6" xr:uid="{68C70BBF-A60F-459D-BFF4-3BFE573DE5CD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Severity"/>
+    <tableColumn id="1" xr3:uid="{BA37A775-A94E-495E-97B9-C78BB0738697}" name="Severity"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="EventClassHashTable" displayName="EventClassHashTable" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{AD0D8A0E-07FC-4F91-AAB2-CCC9BCDE6994}" name="EventClassHashTable" displayName="EventClassHashTable" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{AD0D8A0E-07FC-4F91-AAB2-CCC9BCDE6994}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="EventClassHash"/>
-    <tableColumn id="3" name="TranslationHash"/>
+    <tableColumn id="1" xr3:uid="{9DF2CAD3-9406-4923-BE37-ED41670D6F95}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{6D3217AA-751C-4F05-959D-65E418E9CC72}" name="EventClassHash"/>
+    <tableColumn id="3" xr3:uid="{4F37C865-EF65-4DDD-9DA1-3FDCC1EE1A3E}" name="TranslationHash"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -868,14 +1079,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6B8963-ED32-4C0A-BCEF-2F5666935C79}">
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +1140,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
@@ -937,7 +1148,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
         <v>53</v>
@@ -945,7 +1156,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -953,7 +1164,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -961,7 +1172,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
@@ -969,7 +1180,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
@@ -977,35 +1188,147 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>83</v>
-      </c>
-      <c r="E8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
         <v>85</v>
-      </c>
-      <c r="E9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
         <v>87</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>88</v>
       </c>
-      <c r="E10" t="s">
-        <v>89</v>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1018,11 +1341,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580899C6-FC38-4E30-BA64-5AE6683CAE9E}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,278 +1376,35 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" t="s">
-        <v>116</v>
-      </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
         <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="100.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1333,29 +1413,36 @@
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Helper!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>C1:C15</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{3FDCA0B9-DF35-4E60-A7FC-1A43F4DEA93A}">
+            <xm:f>MATCH(D2,Translations!$A$2:$A$1000,0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D2</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B49C75-BC2F-48D5-A8AF-F79137BE29D1}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,21 +1489,22 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
+        <v>20</v>
+      </c>
+      <c r="D3" t="str" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P1),LEN(CELL("filename",P1))-FIND("]",CELL("filename",P1))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_JogError</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1424,22 +1512,189 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
+      <c r="D4" t="str" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P2),LEN(CELL("filename",P2))-FIND("]",CELL("filename",P2))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_PowerError</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="str" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P3),LEN(CELL("filename",P3))-FIND("]",CELL("filename",P3))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_ResetError</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P4),LEN(CELL("filename",P4))-FIND("]",CELL("filename",P4))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_MoveAbsoluteError</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="str" cm="1">
+        <f t="array" aca="1" ref="D7" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P5),LEN(CELL("filename",P5))-FIND("]",CELL("filename",P5))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_MoveVelocityError</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="str" cm="1">
+        <f t="array" aca="1" ref="D8" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P6),LEN(CELL("filename",P6))-FIND("]",CELL("filename",P6))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_MoveRelativeError</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="str" cm="1">
+        <f t="array" aca="1" ref="D9" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P7),LEN(CELL("filename",P7))-FIND("]",CELL("filename",P7))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_HaltError</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="str" cm="1">
+        <f t="array" aca="1" ref="D10" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P8),LEN(CELL("filename",P8))-FIND("]",CELL("filename",P8))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_StopError</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="str" cm="1">
+        <f t="array" aca="1" ref="D11" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P9),LEN(CELL("filename",P9))-FIND("]",CELL("filename",P9))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_HomeError</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="str" cm="1">
+        <f t="array" aca="1" ref="D12" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P10),LEN(CELL("filename",P10))-FIND("]",CELL("filename",P10))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_GearInError</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
+      <c r="D13" t="str" cm="1">
+        <f t="array" aca="1" ref="D13" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P11),LEN(CELL("filename",P11))-FIND("]",CELL("filename",P11))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_CommandWhileInhibited</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="str" cm="1">
+        <f t="array" aca="1" ref="D14" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P12),LEN(CELL("filename",P12))-FIND("]",CELL("filename",P12))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_DriveError</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="str" cm="1">
+        <f t="array" aca="1" ref="D15" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P13),LEN(CELL("filename",P13))-FIND("]",CELL("filename",P13))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_WriteParameterError</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="str" cm="1">
+        <f t="array" aca="1" ref="D16" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P14),LEN(CELL("filename",P14))-FIND("]",CELL("filename",P14))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_AxisError</v>
       </c>
     </row>
   </sheetData>
@@ -1448,9 +1703,144 @@
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{FD3DCC23-39BB-4683-8102-13F3855F9EAD}">
+            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D3:D16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{C9EF1838-9B86-476F-BE35-CF66F448C978}">
+            <xm:f>MATCH(D2,Translations!$A$2:$A$1000,0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D2</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{079D9DE8-985A-40A8-A15D-D935A08C4988}">
+          <x14:formula1>
+            <xm:f>Helper!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A503A4-4B18-4C4A-B8C4-2EFBD751A220}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="100.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="str" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P1),LEN(CELL("filename",P1))-FIND("]",CELL("filename",P1))),"_Event_", ComponentBase[[#This Row],[Name]])</f>
+        <v>DT_ComponentBase_Event_LogicError</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{A5DC3A9F-D90A-4821-8F45-1CE994861535}">
+            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D3</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7051BEB0-6519-4CB5-84FE-5D40E2AC2065}">
           <x14:formula1>
             <xm:f>Helper!$A$1:$A$6</xm:f>
           </x14:formula1>
@@ -1463,14 +1853,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF848E9-ED7E-45A3-901B-C00D5A5A8427}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,8 +1915,9 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>111</v>
+      <c r="D3" t="str" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P1),LEN(CELL("filename",P1))-FIND("]",CELL("filename",P1))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
+        <v>DT_CylinderBase_Event_ExtendTimeout</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,13 +1930,14 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>112</v>
+      <c r="D4" t="str" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P2),LEN(CELL("filename",P2))-FIND("]",CELL("filename",P2))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
+        <v>DT_CylinderBase_Event_RetractTimeout</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1553,8 +1945,9 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>113</v>
+      <c r="D5" t="str" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P3),LEN(CELL("filename",P3))-FIND("]",CELL("filename",P3))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
+        <v>DT_CylinderBase_Event_InvalidExtendCommand</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,8 +1960,24 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>114</v>
+      <c r="D6" t="str" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P4),LEN(CELL("filename",P4))-FIND("]",CELL("filename",P4))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
+        <v>DT_CylinderBase_Event_InvalidPositionStatus</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="str" cm="1">
+        <f t="array" aca="1" ref="D7" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P5),LEN(CELL("filename",P5))-FIND("]",CELL("filename",P5))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
+        <v>DT_CylinderBase_Event_InvalidRetractCommand</v>
       </c>
     </row>
   </sheetData>
@@ -1577,13 +1986,30 @@
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{54CC6B61-1CAC-4516-BB6B-476FFEBB5B58}">
+            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D3:D7</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{51C79EF2-B637-48A7-ACE0-908184F27E93}">
           <x14:formula1>
             <xm:f>Helper!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C6</xm:sqref>
+          <xm:sqref>C1:C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1592,14 +2018,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F267B193-119A-4564-868A-EEB451CE3AA9}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,8 +2080,9 @@
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>110</v>
+      <c r="D3" t="str" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P1),LEN(CELL("filename",P1))-FIND("]",CELL("filename",P1))),"_Event_", TemplateEventClass[[#This Row],[Name]])</f>
+        <v>DT_TemplateEventClass_Event_Alfa</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,8 +2095,9 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
+      <c r="D4" t="str" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P2),LEN(CELL("filename",P2))-FIND("]",CELL("filename",P2))),"_Event_", TemplateEventClass[[#This Row],[Name]])</f>
+        <v>DT_TemplateEventClass_Event_Bravo</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,19 +2110,38 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
+      <c r="D5" t="str" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P3),LEN(CELL("filename",P3))-FIND("]",CELL("filename",P3))),"_Event_", TemplateEventClass[[#This Row],[Name]])</f>
+        <v>DT_TemplateEventClass_Event_Charlie</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{FAC6C069-4F09-4F33-880F-A25B0CB0249D}">
+            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D3:D5</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F37356EE-A532-4C1D-B4CE-B5596D310BCF}">
           <x14:formula1>
             <xm:f>Helper!$A$1:$A$6</xm:f>
           </x14:formula1>
@@ -1707,14 +2154,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F440BF-D193-4BAD-9037-4363C4A2178A}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1811,7 +2258,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1824,26 +2271,10 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1855,7 +2286,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D97441-C454-4EF9-8985-F563119E536A}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1904,7 +2335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144428E9-8F7B-4AAF-9C9D-BB096563FA03}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1993,21 +2424,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8">
-        <v>1307912399</v>
+        <v>1428209418</v>
       </c>
       <c r="C8">
-        <v>-1307371275</v>
+        <v>793799383</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9">
-        <v>2117481849</v>
+        <v>-2142062505</v>
       </c>
       <c r="C9">
         <v>-1307371275</v>
@@ -2015,13 +2446,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10">
-        <v>-1880678504</v>
+        <v>-953868042</v>
       </c>
       <c r="C10">
-        <v>-1307371275</v>
+        <v>1657467005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Axis Event message fix
</commit_message>
<xml_diff>
--- a/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
+++ b/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beckhoff_Work\github\PML_Base_PLC\PML_Base_PLC_Project\PLC_PML\Base\02_Components\99_EventDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA135DC-925A-4998-836E-BDCC70B1CD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D3BA1F-D343-4E35-AB11-9E0DE4F663EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6F08738D-B868-432B-9E9C-D786710D19A3}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
   <si>
     <t>Key</t>
   </si>
@@ -312,27 +312,9 @@
     <t>DT_AxisBase_Event_GearingSuccessful</t>
   </si>
   <si>
-    <t>{0} - {1} Axis Gearing successful - Master: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Engranamiento de eje fue exitoso - Maestro: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Drive Error Active - Error Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Error de servovariador de eje activo - Código de error: {2}</t>
-  </si>
-  <si>
     <t>DT_AxisBase_Event_CommandError</t>
   </si>
   <si>
-    <t>{0} - {1} Axis Command Error - Command: {2} Code: {3}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Error de comando de axis - Comando: {2} Código: {3}</t>
-  </si>
-  <si>
     <t>DT_CylinderBase_Event_ExtendTimeout</t>
   </si>
   <si>
@@ -396,51 +378,12 @@
     <t>DT_AxisBase_Event_CommandWhileInhibited</t>
   </si>
   <si>
-    <t>{0} - {1} Axis Jog Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis PowerError - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Reset Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Move Position Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Move Velocity Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Move Relative Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Halt Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Stop Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Home Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis Gearing Error - Code: {2}</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis received a motion command while inhibited</t>
-  </si>
-  <si>
     <t>DT_AxisBase_Event_WriteParameterError</t>
   </si>
   <si>
     <t>DT_AxisBase_Event_AxisError</t>
   </si>
   <si>
-    <t>{0} - {1} Axis failed to write drive parameter</t>
-  </si>
-  <si>
-    <t>{0} - {1} Axis error - Code: {2}</t>
-  </si>
-  <si>
     <t>DT_ComponentBase_Event_LogicError</t>
   </si>
   <si>
@@ -451,6 +394,63 @@
   </si>
   <si>
     <t>InvalidRetractCommand</t>
+  </si>
+  <si>
+    <t>{FFA16537-A7B2-4DDE-9F95-DC168DC53CE8}</t>
+  </si>
+  <si>
+    <t>{C6BB256D-3147-4AB2-AE11-F4E3E862EE2A}</t>
+  </si>
+  <si>
+    <t>{198668E0-5E8B-4DB3-9BC3-F71E6825B03A}</t>
+  </si>
+  <si>
+    <t>{0} - Axis received a motion command while inhibited</t>
+  </si>
+  <si>
+    <t>{0} - Axis failed to write drive parameter</t>
+  </si>
+  <si>
+    <t>{0} - Axis Gearing successful - Master: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Drive Error Active - Error Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Jog Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis PowerError - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Reset Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Move Position Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Move Relative Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Move Velocity Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Halt Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Stop Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Home Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Gearing Error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis error - Code: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Axis Command Error - Command: {1} Code: {2}</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -553,62 +553,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -751,8 +695,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B14" totalsRowShown="0">
-  <autoFilter ref="A1:B14" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B17" totalsRowShown="0">
+  <autoFilter ref="A1:B17" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{04E1E75C-BDF3-4286-A594-63A247B782C9}" name="EventClass"/>
     <tableColumn id="2" xr3:uid="{49FC7EFD-1932-435E-822B-CCCC5B22F180}" name="Guid"/>
@@ -1086,7 +1030,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1084,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
@@ -1148,7 +1092,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>53</v>
@@ -1156,7 +1100,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -1164,7 +1108,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -1172,7 +1116,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
@@ -1180,7 +1124,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
@@ -1191,10 +1135,7 @@
         <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1202,133 +1143,127 @@
         <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1379,7 +1314,7 @@
         <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
         <v>67</v>
@@ -1390,7 +1325,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1401,7 +1336,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
@@ -1669,7 +1604,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1684,7 +1619,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1802,7 +1737,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1937,7 +1872,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1967,7 +1902,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2155,13 +2090,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F440BF-D193-4BAD-9037-4363C4A2178A}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2275,6 +2210,30 @@
       </c>
       <c r="B14" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2427,10 +2386,10 @@
         <v>65</v>
       </c>
       <c r="B8">
-        <v>1428209418</v>
+        <v>441165416</v>
       </c>
       <c r="C8">
-        <v>793799383</v>
+        <v>-662023305</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2438,10 +2397,10 @@
         <v>60</v>
       </c>
       <c r="B9">
-        <v>-2142062505</v>
+        <v>-1936318269</v>
       </c>
       <c r="C9">
-        <v>-1307371275</v>
+        <v>488648577</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2449,10 +2408,10 @@
         <v>63</v>
       </c>
       <c r="B10">
-        <v>-953868042</v>
+        <v>-1155527528</v>
       </c>
       <c r="C10">
-        <v>1657467005</v>
+        <v>-1430480341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some template mods and alarm definition fixes
</commit_message>
<xml_diff>
--- a/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
+++ b/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beckhoff_Work\github\PML_Base_PLC\PML_Base_PLC_Project\PLC_PML\Base\02_Components\99_EventDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D3BA1F-D343-4E35-AB11-9E0DE4F663EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379FE01D-9B7C-4C6A-B4E9-6F9EBA25268A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6F08738D-B868-432B-9E9C-D786710D19A3}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="141">
   <si>
     <t>Key</t>
   </si>
@@ -228,9 +228,6 @@
     <t>{0} - Cylinder Retraction timeout - Exceeded configured limit of {1} ms</t>
   </si>
   <si>
-    <t>{0} - Cylinder Extend command invalid - Retract command already active</t>
-  </si>
-  <si>
     <t>{0} - Cylinder Retract command invalid - Extend command already active</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
     <t>{0} - Cylinder command jitter detected - Command cycled between active/inactive within the configured jitter window of {1} ms</t>
   </si>
   <si>
+    <t>InvalidCommand</t>
+  </si>
+  <si>
     <t>{ABE3BB9E-D5A9-46CB-A7C4-C63FD9C74526}</t>
   </si>
   <si>
@@ -321,12 +321,6 @@
     <t>DT_CylinderBase_Event_RetractTimeout</t>
   </si>
   <si>
-    <t>DT_CylinderBase_Event_InvalidExtendCommand</t>
-  </si>
-  <si>
-    <t>DT_CylinderBase_Event_InvalidRetractCommand</t>
-  </si>
-  <si>
     <t>DT_CylinderBase_Event_InvalidPositionStatus</t>
   </si>
   <si>
@@ -390,10 +384,7 @@
     <t>{0} - Logic error in component - Info: {1}</t>
   </si>
   <si>
-    <t>InvalidExtendCommand</t>
-  </si>
-  <si>
-    <t>InvalidRetractCommand</t>
+    <t>DT_CylinderBase_Event_InvalidCommand</t>
   </si>
   <si>
     <t>{FFA16537-A7B2-4DDE-9F95-DC168DC53CE8}</t>
@@ -451,6 +442,51 @@
   </si>
   <si>
     <t>{0} - Axis Command Error - Command: {1} Code: {2}</t>
+  </si>
+  <si>
+    <t>{A0A75C59-E5C7-4769-8166-6E29C73AE472}</t>
+  </si>
+  <si>
+    <t>{C92747F2-72E6-4A19-A4F5-9D4532588768}</t>
+  </si>
+  <si>
+    <t>BrakeError</t>
+  </si>
+  <si>
+    <t>DT_AxisBase_Event_BrakeError</t>
+  </si>
+  <si>
+    <t>{0} - Axis Brake error  - Code: {1}</t>
+  </si>
+  <si>
+    <t>{15D7883C-DD9C-40A5-8A38-DF8FA616F643}</t>
+  </si>
+  <si>
+    <t>ResetLoopDetected</t>
+  </si>
+  <si>
+    <t>DT_ComponentBase_Event_ResetLoopDetected</t>
+  </si>
+  <si>
+    <t>SimulationWarning</t>
+  </si>
+  <si>
+    <t>DT_ComponentBase_Event_SimulationWarning</t>
+  </si>
+  <si>
+    <t>{0} - Component is in Simulation mode - Hardware will not operate</t>
+  </si>
+  <si>
+    <t>{0} -  Potential reset loop detected - Error bit was set and reset in the same scan - TMC Event ID of Offending Alarm: {1}</t>
+  </si>
+  <si>
+    <t>ResetNotPermitted</t>
+  </si>
+  <si>
+    <t>DT_ComponentBase_Event_ResetNotPermitted</t>
+  </si>
+  <si>
+    <t>{0} - Component Reset requested but not permitted - Check for reset/error loop condition in logic</t>
   </si>
 </sst>
 </file>
@@ -492,63 +528,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -639,8 +619,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DDE1A31E-8826-464A-B75B-4BC6DBC7E2E5}" name="AxisBase" displayName="AxisBase" ref="A1:E16" totalsRowShown="0">
-  <autoFilter ref="A1:E16" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DDE1A31E-8826-464A-B75B-4BC6DBC7E2E5}" name="AxisBase" displayName="AxisBase" ref="A1:E17" totalsRowShown="0">
+  <autoFilter ref="A1:E17" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D060CB76-1862-4F57-AE75-CC75B3AABFA0}" name="Name"/>
     <tableColumn id="2" xr3:uid="{0AAF161B-4C9C-4C3B-9FA7-271D21F8C2FA}" name="Id"/>
@@ -653,8 +633,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E270E38A-7D77-4DC9-83C1-9689DC568038}" name="ComponentBase" displayName="ComponentBase" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E270E38A-7D77-4DC9-83C1-9689DC568038}" name="ComponentBase" displayName="ComponentBase" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{109372AA-4697-4EEE-8B86-398CF9153346}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5ABBF4B5-B987-49AB-9DF1-CD69C5AC9BC6}" name="Name"/>
     <tableColumn id="2" xr3:uid="{21104FFF-24AC-4D97-8BC1-530416949D8E}" name="Id"/>
@@ -695,8 +675,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B17" totalsRowShown="0">
-  <autoFilter ref="A1:B17" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B20" totalsRowShown="0">
+  <autoFilter ref="A1:B20" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{04E1E75C-BDF3-4286-A594-63A247B782C9}" name="EventClass"/>
     <tableColumn id="2" xr3:uid="{49FC7EFD-1932-435E-822B-CCCC5B22F180}" name="Guid"/>
@@ -1024,13 +1004,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6B8963-ED32-4C0A-BCEF-2F5666935C79}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1080,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -1108,7 +1088,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -1116,7 +1096,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
@@ -1124,146 +1104,170 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
         <v>105</v>
-      </c>
-      <c r="C23" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1314,7 +1318,7 @@
         <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
         <v>67</v>
@@ -1325,7 +1329,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1336,7 +1340,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
@@ -1371,13 +1375,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B49C75-BC2F-48D5-A8AF-F79137BE29D1}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15:D16"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1608,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1619,7 +1623,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1630,6 +1634,21 @@
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P14),LEN(CELL("filename",P14))-FIND("]",CELL("filename",P14))),"_Event_", AxisBase[[#This Row],[Name]])</f>
         <v>DT_AxisBase_Event_AxisError</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="str" cm="1">
+        <f t="array" aca="1" ref="D17" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P15),LEN(CELL("filename",P15))-FIND("]",CELL("filename",P15))),"_Event_", AxisBase[[#This Row],[Name]])</f>
+        <v>DT_AxisBase_Event_BrakeError</v>
       </c>
     </row>
   </sheetData>
@@ -1642,19 +1661,6 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="2" id="{FD3DCC23-39BB-4683-8102-13F3855F9EAD}">
-            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D3:D16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{C9EF1838-9B86-476F-BE35-CF66F448C978}">
             <xm:f>MATCH(D2,Translations!$A$2:$A$1000,0)</xm:f>
             <x14:dxf>
               <fill>
@@ -1664,7 +1670,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D2</xm:sqref>
+          <xm:sqref>D2:D17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1674,7 +1680,7 @@
           <x14:formula1>
             <xm:f>Helper!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C16</xm:sqref>
+          <xm:sqref>C1:C17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1684,13 +1690,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A503A4-4B18-4C4A-B8C4-2EFBD751A220}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,7 +1743,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1748,6 +1754,51 @@
       <c r="D3" t="str" cm="1">
         <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P1),LEN(CELL("filename",P1))-FIND("]",CELL("filename",P1))),"_Event_", ComponentBase[[#This Row],[Name]])</f>
         <v>DT_ComponentBase_Event_LogicError</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="str" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P2),LEN(CELL("filename",P2))-FIND("]",CELL("filename",P2))),"_Event_", ComponentBase[[#This Row],[Name]])</f>
+        <v>DT_ComponentBase_Event_ResetLoopDetected</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="str" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P3),LEN(CELL("filename",P3))-FIND("]",CELL("filename",P3))),"_Event_", ComponentBase[[#This Row],[Name]])</f>
+        <v>DT_ComponentBase_Event_SimulationWarning</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P4),LEN(CELL("filename",P4))-FIND("]",CELL("filename",P4))),"_Event_", ComponentBase[[#This Row],[Name]])</f>
+        <v>DT_ComponentBase_Event_ResetNotPermitted</v>
       </c>
     </row>
   </sheetData>
@@ -1769,7 +1820,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D3</xm:sqref>
+          <xm:sqref>D3:D6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1779,7 +1830,7 @@
           <x14:formula1>
             <xm:f>Helper!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C5</xm:sqref>
+          <xm:sqref>C1:C6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1789,13 +1840,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF848E9-ED7E-45A3-901B-C00D5A5A8427}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,7 +1923,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1882,7 +1933,7 @@
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P3),LEN(CELL("filename",P3))-FIND("]",CELL("filename",P3))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
-        <v>DT_CylinderBase_Event_InvalidExtendCommand</v>
+        <v>DT_CylinderBase_Event_InvalidCommand</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,21 +1949,6 @@
       <c r="D6" t="str" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P4),LEN(CELL("filename",P4))-FIND("]",CELL("filename",P4))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
         <v>DT_CylinderBase_Event_InvalidPositionStatus</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="str" cm="1">
-        <f t="array" aca="1" ref="D7" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P5),LEN(CELL("filename",P5))-FIND("]",CELL("filename",P5))),"_Event_", CylinderBase[[#This Row],[Name]])</f>
-        <v>DT_CylinderBase_Event_InvalidRetractCommand</v>
       </c>
     </row>
   </sheetData>
@@ -2090,7 +2126,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F440BF-D193-4BAD-9037-4363C4A2178A}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2217,7 +2253,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2234,6 +2270,30 @@
       </c>
       <c r="B17" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2386,10 +2446,10 @@
         <v>65</v>
       </c>
       <c r="B8">
-        <v>441165416</v>
+        <v>1030718497</v>
       </c>
       <c r="C8">
-        <v>-662023305</v>
+        <v>1881079980</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2408,10 +2468,10 @@
         <v>63</v>
       </c>
       <c r="B10">
-        <v>-1155527528</v>
+        <v>1905138439</v>
       </c>
       <c r="C10">
-        <v>-1430480341</v>
+        <v>1332898684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Component event definitions
</commit_message>
<xml_diff>
--- a/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
+++ b/PML_Base_PLC_Project/PLC_PML/Base/02_Components/99_EventDefinitions/BasicComponents_AlarmDefinitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beckhoff_Work\github\PML_Base_PLC\PML_Base_PLC_Project\PLC_PML\Base\02_Components\99_EventDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beckhoff_Work\github\PML_Base_PLC_BenS_Development\PML_Base_PLC_Project\PLC_PML\Base\02_Components\99_EventDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379FE01D-9B7C-4C6A-B4E9-6F9EBA25268A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4009FE1-3277-4175-AF1A-4153CB6331FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6F08738D-B868-432B-9E9C-D786710D19A3}"/>
+    <workbookView xWindow="13680" yWindow="3390" windowWidth="11520" windowHeight="11505" activeTab="2" xr2:uid="{6F08738D-B868-432B-9E9C-D786710D19A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="142">
   <si>
     <t>Key</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>{0} - Component Reset requested but not permitted - Check for reset/error loop condition in logic</t>
+  </si>
+  <si>
+    <t>{949BE30B-68A6-4B8A-A0FC-EB2D4E8C88D9}</t>
   </si>
 </sst>
 </file>
@@ -528,39 +531,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFC8C8"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFC8C8"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFC8C8"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFC8C8"/>
         </patternFill>
       </fill>
     </dxf>
@@ -573,6 +569,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC8C8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -675,8 +676,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B20" totalsRowShown="0">
-  <autoFilter ref="A1:B20" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B21" totalsRowShown="0">
+  <autoFilter ref="A1:B21" xr:uid="{848CB48C-3D90-4BAC-9A20-8997926E4AF3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{04E1E75C-BDF3-4286-A594-63A247B782C9}" name="EventClass"/>
     <tableColumn id="2" xr3:uid="{49FC7EFD-1932-435E-822B-CCCC5B22F180}" name="Guid"/>
@@ -1006,11 +1007,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6B8963-ED32-4C0A-BCEF-2F5666935C79}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1330,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1377,11 +1378,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B49C75-BC2F-48D5-A8AF-F79137BE29D1}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,17 +1661,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{FD3DCC23-39BB-4683-8102-13F3855F9EAD}">
-            <xm:f>MATCH(D2,Translations!$A$2:$A$1000,0)</xm:f>
+          <x14:cfRule type="expression" priority="1" id="{F0F2F44C-AE44-4768-8AEF-BADD0A45FECD}">
+            <xm:f>IF(IFERROR(MATCH(D3,Translations!$A$2:$A$1000,0),FALSE),FALSE,TRUE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
+                  <bgColor rgb="FFFFC8C8"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D2:D17</xm:sqref>
+          <xm:sqref>D3:D17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1690,13 +1691,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A503A4-4B18-4C4A-B8C4-2EFBD751A220}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,6 +1802,12 @@
         <v>DT_ComponentBase_Event_ResetNotPermitted</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f ca="1">MATCH(D3,Translations!$A$2:$A$1000,0)</f>
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1810,12 +1817,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{A5DC3A9F-D90A-4821-8F45-1CE994861535}">
-            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
+          <x14:cfRule type="expression" priority="1" id="{89F96CE8-DB62-4E55-AD1E-118956CAE7E3}">
+            <xm:f>IF(IFERROR(MATCH(D3,Translations!$A$2:$A$1000,0),FALSE),FALSE,TRUE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
+                  <bgColor rgb="FFFFC8C8"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -1825,7 +1832,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7051BEB0-6519-4CB5-84FE-5D40E2AC2065}">
           <x14:formula1>
             <xm:f>Helper!$A$1:$A$6</xm:f>
@@ -1846,7 +1853,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,17 +1967,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{54CC6B61-1CAC-4516-BB6B-476FFEBB5B58}">
-            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
+          <x14:cfRule type="expression" priority="1" id="{46FDACA3-9FBA-421A-A61A-59875A3591ED}">
+            <xm:f>IF(IFERROR(MATCH(D3,Translations!$A$2:$A$1000,0),FALSE),FALSE,TRUE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
+                  <bgColor rgb="FFFFC8C8"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D3:D7</xm:sqref>
+          <xm:sqref>D3:D6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2097,11 +2104,11 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{FAC6C069-4F09-4F33-880F-A25B0CB0249D}">
-            <xm:f>MATCH(D3,Translations!$A$2:$A$1000,0)</xm:f>
+            <xm:f>IF(IFERROR(MATCH(D3,Translations!$A$2:$A$1000,0),FALSE),FALSE,TRUE)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
+                  <bgColor rgb="FFFFC8C8"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -2126,7 +2133,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F440BF-D193-4BAD-9037-4363C4A2178A}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2294,6 +2301,14 @@
       </c>
       <c r="B20" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2457,10 +2472,10 @@
         <v>60</v>
       </c>
       <c r="B9">
-        <v>-1936318269</v>
+        <v>507357128</v>
       </c>
       <c r="C9">
-        <v>488648577</v>
+        <v>-287402201</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>